<commit_message>
Updated with grabbing values
</commit_message>
<xml_diff>
--- a/DataDrivenExecl/DemoData.xlsx
+++ b/DataDrivenExecl/DemoData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium file\ExcelDataDriven\GitHub\ExceldataDriven\DataDrivenExecl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D424528-7A0F-4FCB-8E6C-BCD7ABFB0D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F9A3D2B-B5E8-42F2-A5D6-BE9BFF10852D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="-210" windowWidth="15375" windowHeight="7875" xr2:uid="{E2D4D9F4-E7A6-464B-96B2-8B88C87E814D}"/>
+    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" xr2:uid="{E2D4D9F4-E7A6-464B-96B2-8B88C87E814D}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData1" sheetId="1" r:id="rId1"/>
     <sheet name="TestData2" sheetId="2" r:id="rId2"/>
     <sheet name="TestData3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -450,7 +450,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Handle with numeric value
</commit_message>
<xml_diff>
--- a/DataDrivenExecl/DemoData.xlsx
+++ b/DataDrivenExecl/DemoData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium file\ExcelDataDriven\GitHub\ExceldataDriven\DataDrivenExecl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F9A3D2B-B5E8-42F2-A5D6-BE9BFF10852D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF27DCF-8AAA-4C7F-8376-7216D7491B8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" xr2:uid="{E2D4D9F4-E7A6-464B-96B2-8B88C87E814D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TestCases</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>ijkl</t>
-  </si>
-  <si>
-    <t>Sup</t>
   </si>
   <si>
     <t>Sup1</t>
@@ -450,7 +447,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,14 +504,14 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,13 +519,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated printing with excel
</commit_message>
<xml_diff>
--- a/DataDrivenExecl/DemoData.xlsx
+++ b/DataDrivenExecl/DemoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Selenium file\ExcelDataDriven\GitHub\ExceldataDriven\DataDrivenExecl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF27DCF-8AAA-4C7F-8376-7216D7491B8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBE912E-77D5-4B94-9D5C-5ACC49CEB04B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" xr2:uid="{E2D4D9F4-E7A6-464B-96B2-8B88C87E814D}"/>
+    <workbookView xWindow="5115" yWindow="0" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E2D4D9F4-E7A6-464B-96B2-8B88C87E814D}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>TestCases</t>
   </si>
@@ -93,6 +93,81 @@
   </si>
   <si>
     <t>ijk</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>Value4</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Value5</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -446,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941B7C0E-3576-4EE3-81DE-B741355AA8FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -535,12 +610,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4CBB22-7A46-4ED1-9C37-D67F9665F949}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>